<commit_message>
Removing Latin1 non-breaking space unicode
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuhnsa/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/biowulf2DME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFAA425C-8B28-E446-8A49-8A0A7AFD583D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D9752-544A-C144-A6C8-A9E5C0AD8430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8740" yWindow="460" windowWidth="29600" windowHeight="20300" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -5293,9 +5293,6 @@
     <t>Lung</t>
   </si>
   <si>
-    <t>Squamous cell carcinoma (SCC)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Age of the sample before extraction. </t>
     </r>
@@ -5386,6 +5383,9 @@
   </si>
   <si>
     <t>Novogene</t>
+  </si>
+  <si>
+    <t>Squamous cell carcinoma (SCC)</t>
   </si>
 </sst>
 </file>
@@ -6141,8 +6141,8 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="E65" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6862,7 +6862,7 @@
         <v>478</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="D43" s="43" t="s">
         <v>1548</v>
@@ -7090,7 +7090,7 @@
         <v>1566</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17">
@@ -7107,7 +7107,7 @@
         <v>1567</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1587</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17">
@@ -7121,7 +7121,7 @@
         <v>1522</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="34">
@@ -7152,10 +7152,10 @@
         <v>1523</v>
       </c>
       <c r="D60" s="43" t="s">
+        <v>1587</v>
+      </c>
+      <c r="E60" s="43" t="s">
         <v>1588</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>1589</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17">
@@ -7169,7 +7169,7 @@
         <v>1524</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17">
@@ -7183,10 +7183,10 @@
         <v>1525</v>
       </c>
       <c r="D62" s="43" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>1580</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>1581</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17">
@@ -7200,10 +7200,10 @@
         <v>1526</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17">
@@ -7217,10 +7217,10 @@
         <v>1527</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17">
@@ -7234,10 +7234,10 @@
         <v>1528</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>1569</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17">
@@ -7251,10 +7251,10 @@
         <v>1529</v>
       </c>
       <c r="D66" s="43" t="s">
+        <v>1569</v>
+      </c>
+      <c r="E66" s="43" t="s">
         <v>1570</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>1571</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17">
@@ -7268,10 +7268,10 @@
         <v>1530</v>
       </c>
       <c r="D67" s="43" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" customHeight="1">
@@ -7285,10 +7285,10 @@
         <v>1532</v>
       </c>
       <c r="D68" s="43" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17">
@@ -7302,7 +7302,7 @@
         <v>1533</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="E69" s="64">
         <v>20814</v>
@@ -7319,7 +7319,7 @@
         <v>1534</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
   </sheetData>
@@ -7479,7 +7479,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -8285,7 +8285,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -24297,7 +24297,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>

</xml_diff>

<commit_message>
Adding data catalogue parser and merging PI cells in template spreadsheet
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/biowulf2DME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18D9752-544A-C144-A6C8-A9E5C0AD8430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE85D8C-7020-A740-885B-AA68F557F5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-29620" yWindow="-6700" windowWidth="29600" windowHeight="28340" activeTab="4" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -5643,7 +5643,7 @@
     <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -5810,6 +5810,9 @@
     </xf>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -6141,8 +6144,8 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7341,7 +7344,7 @@
   <dimension ref="A1:E38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -7385,13 +7388,17 @@
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="75"/>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="75"/>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" spans="1:4" ht="16">
       <c r="A6" s="6" t="s">
@@ -7614,7 +7621,7 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B3:D3"/>
@@ -7622,6 +7629,8 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12" xr:uid="{737CDC18-C3D0-BF4D-A0F8-A73EC80A82CA}">
@@ -8110,7 +8119,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -8154,17 +8163,21 @@
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="75" t="s">
         <v>100</v>
       </c>
+      <c r="C4" s="75"/>
+      <c r="D4" s="75"/>
     </row>
     <row r="5" spans="1:4" ht="16">
       <c r="A5" s="7" t="s">
         <v>403</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="75" t="s">
         <v>367</v>
       </c>
+      <c r="C5" s="75"/>
+      <c r="D5" s="75"/>
     </row>
     <row r="6" spans="1:4" ht="16">
       <c r="A6" s="6" t="s">
@@ -8451,7 +8464,7 @@
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
   <dataConsolidate/>
-  <mergeCells count="7">
+  <mergeCells count="9">
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="B3:D3"/>
@@ -8459,6 +8472,8 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="B17:D17"/>
     <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B5:D5"/>
   </mergeCells>
   <dataValidations count="8">
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Error: Invalid email" error="Please enter a vaild point-of-contact email address." sqref="B18" xr:uid="{F72E01BC-109B-5B4F-A841-048577AA2E55}">
@@ -8552,7 +8567,7 @@
   </sheetPr>
   <dimension ref="A1:Z430"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A449" sqref="A449"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updating PI collection name
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/biowulf2DME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CE85D8C-7020-A740-885B-AA68F557F5DC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E840398-C991-3F4B-B76C-A0AEFD0C699B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29620" yWindow="-6700" windowWidth="29600" windowHeight="28340" activeTab="4" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -4332,9 +4332,6 @@
   </si>
   <si>
     <t>Project Collection</t>
-  </si>
-  <si>
-    <t>PI Collection</t>
   </si>
   <si>
     <t>Example</t>
@@ -5386,6 +5383,9 @@
   </si>
   <si>
     <t>Squamous cell carcinoma (SCC)</t>
+  </si>
+  <si>
+    <t>PI_Lab Collection</t>
   </si>
 </sst>
 </file>
@@ -6144,8 +6144,8 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="K11" sqref="K10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="2" spans="1:11" ht="20">
       <c r="A2" s="46" t="s">
-        <v>1431</v>
+        <v>1592</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>1428</v>
@@ -6182,7 +6182,7 @@
         <v>474</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="F2" s="50"/>
     </row>
@@ -6197,10 +6197,10 @@
         <v>1425</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
@@ -6220,10 +6220,10 @@
         <v>1426</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -6256,7 +6256,7 @@
         <v>474</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
@@ -6273,10 +6273,10 @@
         <v>404</v>
       </c>
       <c r="C7" s="48" t="s">
+        <v>1432</v>
+      </c>
+      <c r="D7" s="43" t="s">
         <v>1433</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>1434</v>
       </c>
       <c r="E7" s="43" t="s">
         <v>13</v>
@@ -6290,10 +6290,10 @@
         <v>408</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="E8" s="43" t="s">
         <v>318</v>
@@ -6307,10 +6307,10 @@
         <v>432</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>409</v>
@@ -6324,10 +6324,10 @@
         <v>5</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="E10" s="43" t="s">
         <v>439</v>
@@ -6341,10 +6341,10 @@
         <v>437</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>444</v>
@@ -6358,10 +6358,10 @@
         <v>435</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="E12" s="22">
         <v>212</v>
@@ -6375,13 +6375,13 @@
         <v>436</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17">
@@ -6392,13 +6392,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="53" customHeight="1">
@@ -6409,10 +6409,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="17">
@@ -6423,13 +6423,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17">
@@ -6440,13 +6440,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="D17" s="43" t="s">
+        <v>1454</v>
+      </c>
+      <c r="E17" s="43" t="s">
         <v>1455</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>1456</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17">
@@ -6457,10 +6457,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="E18" s="59" t="s">
         <v>441</v>
@@ -6468,16 +6468,16 @@
     </row>
     <row r="19" spans="1:5" ht="17">
       <c r="A19" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B19" s="60" t="s">
         <v>456</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="E19" s="62" t="s">
         <v>460</v>
@@ -6485,27 +6485,27 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B20" s="60" t="s">
         <v>438</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17">
       <c r="A21" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B21" s="60" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="E21" s="43" t="s">
         <v>424</v>
@@ -6513,16 +6513,16 @@
     </row>
     <row r="22" spans="1:5" ht="17">
       <c r="A22" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B22" s="60" t="s">
         <v>431</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>1463</v>
+        <v>1462</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="E22" s="22">
         <v>27565351</v>
@@ -6530,67 +6530,67 @@
     </row>
     <row r="23" spans="1:5" ht="17">
       <c r="A23" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B23" s="61" t="s">
         <v>405</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="D23" s="43" t="s">
+        <v>1475</v>
+      </c>
+      <c r="E23" s="43" t="s">
         <v>1476</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>1477</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17">
       <c r="A24" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B24" s="61" t="s">
         <v>452</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="D24" s="43" t="s">
+        <v>1478</v>
+      </c>
+      <c r="E24" s="56" t="s">
         <v>1479</v>
-      </c>
-      <c r="E24" s="56" t="s">
-        <v>1480</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34">
       <c r="A25" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B25" s="60" t="s">
         <v>433</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="D25" s="43" t="s">
+        <v>1480</v>
+      </c>
+      <c r="E25" s="43" t="s">
         <v>1481</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>1482</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34">
       <c r="A26" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B26" s="60" t="s">
         <v>451</v>
       </c>
       <c r="C26" s="48" t="s">
+        <v>1470</v>
+      </c>
+      <c r="D26" s="43" t="s">
         <v>1471</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>1472</v>
       </c>
       <c r="E26" s="43" t="s">
         <v>448</v>
@@ -6598,30 +6598,30 @@
     </row>
     <row r="27" spans="1:5" ht="17">
       <c r="A27" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B27" s="61" t="s">
         <v>429</v>
       </c>
       <c r="C27" s="48" t="s">
+        <v>1472</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>1473</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>1474</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17">
       <c r="A28" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B28" s="60" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="E28" s="43" t="s">
         <v>449</v>
@@ -6629,16 +6629,16 @@
     </row>
     <row r="29" spans="1:5" ht="17">
       <c r="A29" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B29" s="60" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="E29" s="43" t="s">
         <v>450</v>
@@ -6646,36 +6646,36 @@
     </row>
     <row r="30" spans="1:5" ht="17">
       <c r="A30" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B30" s="60" t="s">
         <v>454</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34">
       <c r="A31" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B31" s="60" t="s">
         <v>434</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="D31" s="43" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E31" s="43" t="s">
         <v>1495</v>
-      </c>
-      <c r="E31" s="43" t="s">
-        <v>1496</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -6683,7 +6683,7 @@
     </row>
     <row r="33" spans="1:11" ht="20">
       <c r="A33" s="46" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>1428</v>
@@ -6695,7 +6695,7 @@
         <v>474</v>
       </c>
       <c r="E33" s="57" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="F33" s="52"/>
       <c r="G33" s="52"/>
@@ -6712,13 +6712,13 @@
         <v>465</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D34" s="43" t="s">
+        <v>1535</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>1536</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>1537</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68">
@@ -6729,13 +6729,13 @@
         <v>463</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="17">
@@ -6746,10 +6746,10 @@
         <v>466</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="E36" s="43" t="s">
         <v>318</v>
@@ -6763,30 +6763,30 @@
         <v>491</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" customHeight="1">
       <c r="A38" s="55" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>492</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="17">
@@ -6797,10 +6797,10 @@
         <v>464</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="E39" s="43" t="s">
         <v>495</v>
@@ -6814,10 +6814,10 @@
         <v>475</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="E40" s="43" t="s">
         <v>444</v>
@@ -6828,16 +6828,16 @@
         <v>1429</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17">
@@ -6848,10 +6848,10 @@
         <v>467</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="E42" s="64" t="b">
         <v>1</v>
@@ -6865,10 +6865,10 @@
         <v>478</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>1590</v>
+        <v>1589</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="E43" s="64" t="b">
         <v>0</v>
@@ -6882,10 +6882,10 @@
         <v>489</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="E44" s="64" t="b">
         <v>1</v>
@@ -6899,10 +6899,10 @@
         <v>476</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>521</v>
@@ -6910,33 +6910,33 @@
     </row>
     <row r="46" spans="1:11" ht="17">
       <c r="A46" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B46" s="61" t="s">
         <v>1416</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D46" s="43" t="s">
+        <v>1550</v>
+      </c>
+      <c r="E46" s="67" t="s">
         <v>1551</v>
-      </c>
-      <c r="E46" s="67" t="s">
-        <v>1552</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="17">
       <c r="A47" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="E47" s="68" t="s">
         <v>1419</v>
@@ -6944,84 +6944,84 @@
     </row>
     <row r="48" spans="1:11" ht="17">
       <c r="A48" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B48" s="61" t="s">
         <v>468</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D48" s="43" t="s">
+        <v>1553</v>
+      </c>
+      <c r="E48" s="43" t="s">
         <v>1554</v>
-      </c>
-      <c r="E48" s="43" t="s">
-        <v>1555</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17">
       <c r="A49" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B49" s="61" t="s">
         <v>479</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17">
       <c r="A50" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B50" s="61" t="s">
         <v>488</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="D50" s="43" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21" customHeight="1">
       <c r="A51" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B51" s="61" t="s">
         <v>490</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17">
       <c r="A52" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B52" s="61" t="s">
         <v>454</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
       <c r="E52" t="s">
         <v>1418</v>
@@ -7030,16 +7030,16 @@
     </row>
     <row r="53" spans="1:6" ht="17">
       <c r="A53" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B53" s="61" t="s">
         <v>477</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
       <c r="E53" s="43" t="s">
         <v>1417</v>
@@ -7047,16 +7047,16 @@
     </row>
     <row r="54" spans="1:6" ht="17">
       <c r="A54" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B54" s="61" t="s">
         <v>471</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="E54" s="43" t="s">
         <v>514</v>
@@ -7064,16 +7064,16 @@
     </row>
     <row r="55" spans="1:6" ht="17">
       <c r="A55" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B55" s="61" t="s">
         <v>483</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D55" s="43" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="E55" s="64">
         <v>8.3000000000000007</v>
@@ -7081,231 +7081,231 @@
     </row>
     <row r="56" spans="1:6" ht="69" customHeight="1">
       <c r="A56" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B56" s="61" t="s">
         <v>469</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D56" s="43" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17">
       <c r="A57" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B57" s="61" t="s">
         <v>470</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17">
       <c r="A58" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B58" s="61" t="s">
         <v>480</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="34">
       <c r="A59" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B59" s="61" t="s">
         <v>434</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="D59" s="43" t="s">
+        <v>1494</v>
+      </c>
+      <c r="E59" s="43" t="s">
         <v>1495</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>1496</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17">
       <c r="A60" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B60" s="61" t="s">
         <v>520</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D60" s="43" t="s">
+        <v>1586</v>
+      </c>
+      <c r="E60" s="43" t="s">
         <v>1587</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>1588</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17">
       <c r="A61" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B61" s="61" t="s">
         <v>487</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17">
       <c r="A62" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B62" s="61" t="s">
         <v>472</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="D62" s="43" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>1579</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>1580</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17">
       <c r="A63" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B63" s="61" t="s">
         <v>485</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17">
       <c r="A64" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B64" s="61" t="s">
         <v>519</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17">
       <c r="A65" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B65" s="61" t="s">
         <v>481</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>1592</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17">
       <c r="A66" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B66" s="61" t="s">
         <v>482</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="D66" s="43" t="s">
+        <v>1568</v>
+      </c>
+      <c r="E66" s="43" t="s">
         <v>1569</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>1570</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17">
       <c r="A67" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B67" s="61" t="s">
         <v>484</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="D67" s="43" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" customHeight="1">
       <c r="A68" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B68" s="61" t="s">
+        <v>1530</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>1531</v>
       </c>
-      <c r="C68" s="48" t="s">
-        <v>1532</v>
-      </c>
       <c r="D68" s="43" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17">
       <c r="A69" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B69" s="61" t="s">
         <v>486</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>1589</v>
+        <v>1588</v>
       </c>
       <c r="E69" s="64">
         <v>20814</v>
@@ -7313,16 +7313,16 @@
     </row>
     <row r="70" spans="1:5" ht="17">
       <c r="A70" s="55" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="B70" s="61" t="s">
         <v>517</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
   </sheetData>
@@ -7486,7 +7486,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44063</v>
+        <v>44085</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -7829,7 +7829,7 @@
         <v>475</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>467</v>
@@ -8004,7 +8004,7 @@
         <v>1416</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>468</v>
@@ -8067,7 +8067,7 @@
         <v>484</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>486</v>
@@ -8298,7 +8298,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44063</v>
+        <v>44085</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -8446,7 +8446,7 @@
         <v>1415</v>
       </c>
       <c r="C32" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="16">
@@ -8567,7 +8567,7 @@
   </sheetPr>
   <dimension ref="A1:Z430"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A449" sqref="A449"/>
     </sheetView>
   </sheetViews>
@@ -8678,7 +8678,7 @@
         <v>475</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>467</v>
@@ -16790,7 +16790,7 @@
         <v>1416</v>
       </c>
       <c r="C218" s="32" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D218" s="15" t="s">
         <v>468</v>
@@ -16853,7 +16853,7 @@
         <v>484</v>
       </c>
       <c r="X218" s="2" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="Y218" s="2" t="s">
         <v>486</v>
@@ -24312,7 +24312,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1591</v>
+        <v>1590</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>

</xml_diff>

<commit_message>
Removing date auto-resolver for user template
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/biowulf2DME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E840398-C991-3F4B-B76C-A0AEFD0C699B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{852C2B55-DF27-B949-8370-1C54EF8FADDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" activeTab="1" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -6144,8 +6144,8 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="K11" sqref="K10:K11"/>
+    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -7343,8 +7343,8 @@
   </sheetPr>
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19"/>
@@ -7484,10 +7484,7 @@
       <c r="A16" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="72">
-        <f ca="1">TODAY()</f>
-        <v>44085</v>
-      </c>
+      <c r="B16" s="72"/>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
     </row>
@@ -7632,7 +7629,7 @@
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
   </mergeCells>
-  <dataValidations count="8">
+  <dataValidations count="9">
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B12:D12" xr:uid="{737CDC18-C3D0-BF4D-A0F8-A73EC80A82CA}">
       <formula1>-1</formula1>
       <formula2>1000000</formula2>
@@ -7655,6 +7652,7 @@
     <dataValidation type="custom" showInputMessage="1" showErrorMessage="1" errorTitle="Error: Invalid email" error="Please enter a vaild point-of-contact email address." sqref="B18" xr:uid="{97F796C5-377B-B244-AC2C-05FEE0C6DE77}">
       <formula1>ISNUMBER(MATCH("*@*.?*",B18,0))</formula1>
     </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter a start date in the following format:_x000a_YYYY-MM-DD" sqref="A16" xr:uid="{36E2BF9A-0407-1A48-B7BD-F1BD8A59B705}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -8298,7 +8296,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44085</v>
+        <v>44088</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>

</xml_diff>

<commit_message>
Updating DME field name
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/ccbr1099/biowulf2DME/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DME/biowulf2DME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F393F7-A8D6-0946-A334-639529149CE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4C8070-422E-4443-85F0-7FDC7A5C6AAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" activeTab="3" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -4772,9 +4772,6 @@
   </si>
   <si>
     <t>sample_name</t>
-  </si>
-  <si>
-    <t>sequencing_appplication_type</t>
   </si>
   <si>
     <t>file_type</t>
@@ -5368,6 +5365,9 @@
   </si>
   <si>
     <t>PI_Lab Collection</t>
+  </si>
+  <si>
+    <t>sequencing_application_type</t>
   </si>
 </sst>
 </file>
@@ -6126,8 +6126,8 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6152,7 +6152,7 @@
     </row>
     <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>1423</v>
@@ -6697,10 +6697,10 @@
         <v>1493</v>
       </c>
       <c r="D34" s="43" t="s">
+        <v>1528</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>1529</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>1530</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -6714,10 +6714,10 @@
         <v>1494</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6728,7 +6728,7 @@
         <v>461</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1495</v>
+        <v>1586</v>
       </c>
       <c r="D36" s="43" t="s">
         <v>1443</v>
@@ -6745,30 +6745,30 @@
         <v>486</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="55" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>487</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6779,10 +6779,10 @@
         <v>459</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="E39" s="43" t="s">
         <v>490</v>
@@ -6796,10 +6796,10 @@
         <v>470</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E40" s="43" t="s">
         <v>444</v>
@@ -6813,13 +6813,13 @@
         <v>1490</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6830,10 +6830,10 @@
         <v>462</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="E42" s="64" t="b">
         <v>1</v>
@@ -6847,10 +6847,10 @@
         <v>473</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="E43" s="64" t="b">
         <v>0</v>
@@ -6864,10 +6864,10 @@
         <v>484</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="E44" s="64" t="b">
         <v>1</v>
@@ -6881,10 +6881,10 @@
         <v>471</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>516</v>
@@ -6898,13 +6898,13 @@
         <v>1411</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D46" s="43" t="s">
+        <v>1543</v>
+      </c>
+      <c r="E46" s="67" t="s">
         <v>1544</v>
-      </c>
-      <c r="E46" s="67" t="s">
-        <v>1545</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6915,10 +6915,10 @@
         <v>1491</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="E47" s="68" t="s">
         <v>1414</v>
@@ -6932,13 +6932,13 @@
         <v>463</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D48" s="43" t="s">
+        <v>1546</v>
+      </c>
+      <c r="E48" s="43" t="s">
         <v>1547</v>
-      </c>
-      <c r="E48" s="43" t="s">
-        <v>1548</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6949,13 +6949,13 @@
         <v>474</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6966,13 +6966,13 @@
         <v>483</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="D50" s="43" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -6983,13 +6983,13 @@
         <v>485</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7003,7 +7003,7 @@
         <v>1480</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="E52" t="s">
         <v>1413</v>
@@ -7018,10 +7018,10 @@
         <v>472</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E53" s="43" t="s">
         <v>1412</v>
@@ -7035,10 +7035,10 @@
         <v>466</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="E54" s="43" t="s">
         <v>509</v>
@@ -7052,10 +7052,10 @@
         <v>478</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="D55" s="43" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E55" s="64">
         <v>8.3000000000000007</v>
@@ -7069,13 +7069,13 @@
         <v>464</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="D56" s="43" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7086,13 +7086,13 @@
         <v>465</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7103,10 +7103,10 @@
         <v>475</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -7134,13 +7134,13 @@
         <v>515</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="D60" s="43" t="s">
+        <v>1579</v>
+      </c>
+      <c r="E60" s="43" t="s">
         <v>1580</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>1581</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7151,10 +7151,10 @@
         <v>482</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7165,13 +7165,13 @@
         <v>467</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="D62" s="43" t="s">
+        <v>1571</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>1572</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>1573</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7182,13 +7182,13 @@
         <v>480</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7199,13 +7199,13 @@
         <v>514</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7216,13 +7216,13 @@
         <v>476</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7233,13 +7233,13 @@
         <v>477</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D66" s="43" t="s">
+        <v>1561</v>
+      </c>
+      <c r="E66" s="43" t="s">
         <v>1562</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>1563</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7250,13 +7250,13 @@
         <v>479</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D67" s="43" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7264,16 +7264,16 @@
         <v>1438</v>
       </c>
       <c r="B68" s="61" t="s">
+        <v>1523</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>1524</v>
       </c>
-      <c r="C68" s="48" t="s">
-        <v>1525</v>
-      </c>
       <c r="D68" s="43" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7284,10 +7284,10 @@
         <v>481</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="E69" s="64">
         <v>20814</v>
@@ -7301,10 +7301,10 @@
         <v>512</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
   </sheetData>
@@ -8047,7 +8047,7 @@
         <v>479</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>481</v>
@@ -8098,7 +8098,7 @@
   </sheetPr>
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44222</v>
+        <v>44223</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -16803,7 +16803,7 @@
         <v>479</v>
       </c>
       <c r="X218" s="2" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="Y218" s="2" t="s">
         <v>481</v>
@@ -24262,7 +24262,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>

</xml_diff>

<commit_message>
Adding data vailation rule to enforce date format and range
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DME/biowulf2DME/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C4C8070-422E-4443-85F0-7FDC7A5C6AAC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFFFD6E-F7E9-2D4A-B1B9-AD8ADEFE02AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
@@ -4778,9 +4778,6 @@
   </si>
   <si>
     <t>source_organism</t>
-  </si>
-  <si>
-    <t>tissue_type</t>
   </si>
   <si>
     <t>is_tumor</t>
@@ -5368,6 +5365,9 @@
   </si>
   <si>
     <t>sequencing_application_type</t>
+  </si>
+  <si>
+    <t>sample_type</t>
   </si>
 </sst>
 </file>
@@ -6127,7 +6127,7 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6152,7 +6152,7 @@
     </row>
     <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>1423</v>
@@ -6697,10 +6697,10 @@
         <v>1493</v>
       </c>
       <c r="D34" s="43" t="s">
+        <v>1527</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>1528</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>1529</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -6714,10 +6714,10 @@
         <v>1494</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6728,7 +6728,7 @@
         <v>461</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D36" s="43" t="s">
         <v>1443</v>
@@ -6745,30 +6745,30 @@
         <v>486</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="55" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>487</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6782,7 +6782,7 @@
         <v>1495</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E39" s="43" t="s">
         <v>490</v>
@@ -6799,7 +6799,7 @@
         <v>1496</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="E40" s="43" t="s">
         <v>444</v>
@@ -6813,13 +6813,13 @@
         <v>1490</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>1497</v>
+        <v>1586</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6830,10 +6830,10 @@
         <v>462</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="E42" s="64" t="b">
         <v>1</v>
@@ -6847,10 +6847,10 @@
         <v>473</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="E43" s="64" t="b">
         <v>0</v>
@@ -6864,10 +6864,10 @@
         <v>484</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="E44" s="64" t="b">
         <v>1</v>
@@ -6881,10 +6881,10 @@
         <v>471</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>516</v>
@@ -6898,13 +6898,13 @@
         <v>1411</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D46" s="43" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E46" s="67" t="s">
         <v>1543</v>
-      </c>
-      <c r="E46" s="67" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6915,10 +6915,10 @@
         <v>1491</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="E47" s="68" t="s">
         <v>1414</v>
@@ -6932,13 +6932,13 @@
         <v>463</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="D48" s="43" t="s">
+        <v>1545</v>
+      </c>
+      <c r="E48" s="43" t="s">
         <v>1546</v>
-      </c>
-      <c r="E48" s="43" t="s">
-        <v>1547</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6949,13 +6949,13 @@
         <v>474</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -6966,13 +6966,13 @@
         <v>483</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="D50" s="43" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
@@ -6983,13 +6983,13 @@
         <v>485</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7003,7 +7003,7 @@
         <v>1480</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="E52" t="s">
         <v>1413</v>
@@ -7018,10 +7018,10 @@
         <v>472</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="E53" s="43" t="s">
         <v>1412</v>
@@ -7035,10 +7035,10 @@
         <v>466</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="E54" s="43" t="s">
         <v>509</v>
@@ -7052,10 +7052,10 @@
         <v>478</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D55" s="43" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
       <c r="E55" s="64">
         <v>8.3000000000000007</v>
@@ -7069,13 +7069,13 @@
         <v>464</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="D56" s="43" t="s">
-        <v>1558</v>
+        <v>1557</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>1577</v>
+        <v>1576</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7086,13 +7086,13 @@
         <v>465</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>1559</v>
+        <v>1558</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7103,10 +7103,10 @@
         <v>475</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>1576</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="34" x14ac:dyDescent="0.2">
@@ -7134,13 +7134,13 @@
         <v>515</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D60" s="43" t="s">
+        <v>1578</v>
+      </c>
+      <c r="E60" s="43" t="s">
         <v>1579</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>1580</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7151,10 +7151,10 @@
         <v>482</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7165,13 +7165,13 @@
         <v>467</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="D62" s="43" t="s">
+        <v>1570</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>1571</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>1572</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7182,13 +7182,13 @@
         <v>480</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -7199,13 +7199,13 @@
         <v>514</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>1568</v>
+        <v>1567</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7216,13 +7216,13 @@
         <v>476</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7233,13 +7233,13 @@
         <v>477</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="D66" s="43" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E66" s="43" t="s">
         <v>1561</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>1562</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7250,13 +7250,13 @@
         <v>479</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D67" s="43" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
@@ -7264,16 +7264,16 @@
         <v>1438</v>
       </c>
       <c r="B68" s="61" t="s">
+        <v>1522</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>1523</v>
       </c>
-      <c r="C68" s="48" t="s">
-        <v>1524</v>
-      </c>
       <c r="D68" s="43" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -7284,10 +7284,10 @@
         <v>481</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="E69" s="64">
         <v>20814</v>
@@ -7301,10 +7301,10 @@
         <v>512</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
     </row>
   </sheetData>
@@ -7623,10 +7623,6 @@
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B6" xr:uid="{1266F5D0-3163-F048-B27C-CFC77D986EB7}">
       <formula1>"Project"</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B16" xr:uid="{FBB7BF57-5353-2D43-9516-22E71EAC58F8}">
-      <formula1>TODAY()-548</formula1>
-      <formula2>TODAY()+548</formula2>
-    </dataValidation>
     <dataValidation type="list" showDropDown="1" showInputMessage="1" showErrorMessage="1" sqref="B3" xr:uid="{C4B76B06-5B97-C546-9ADF-09E0B9EF06FF}">
       <formula1>"PI_Lab"</formula1>
     </dataValidation>
@@ -7635,6 +7631,10 @@
       <formula1>ISNUMBER(MATCH("*@*.?*",B18,0))</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Please enter a start date in the following format:_x000a_YYYY-MM-DD" sqref="A16" xr:uid="{36E2BF9A-0407-1A48-B7BD-F1BD8A59B705}"/>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid Date" error="Please enter a date in YYYY-MM-DD format." sqref="B16:D16" xr:uid="{C47C6BBA-462F-504C-B591-F46F59E91B6D}">
+      <formula1>TODAY()-548</formula1>
+      <formula2>TODAY()+548</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -8047,7 +8047,7 @@
         <v>479</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>481</v>
@@ -8517,7 +8517,7 @@
   </sheetPr>
   <dimension ref="A1:Z430"/>
   <sheetViews>
-    <sheetView topLeftCell="A74" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A449" sqref="A449"/>
     </sheetView>
   </sheetViews>
@@ -16803,7 +16803,7 @@
         <v>479</v>
       </c>
       <c r="X218" s="2" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="Y218" s="2" t="s">
         <v>481</v>
@@ -24262,7 +24262,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>

</xml_diff>

<commit_message>
Updating DME metadata to be harmonized with SF
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DME/biowulf2DME/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuhnsa/Desktop/Archive/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFFFD6E-F7E9-2D4A-B1B9-AD8ADEFE02AB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{93188DA8-CE5D-334A-9143-EF0909ACDEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29620" yWindow="-6740" windowWidth="29600" windowHeight="28340" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-23440" yWindow="-28340" windowWidth="35840" windowHeight="26680" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -4344,12 +4344,6 @@
   </si>
   <si>
     <t>summary_of_samples</t>
-  </si>
-  <si>
-    <t>start_date</t>
-  </si>
-  <si>
-    <t>project_poc</t>
   </si>
   <si>
     <t>poc_email</t>
@@ -5368,6 +5362,12 @@
   </si>
   <si>
     <t>sample_type</t>
+  </si>
+  <si>
+    <t>contact_name</t>
+  </si>
+  <si>
+    <t>project_start_date</t>
   </si>
 </sst>
 </file>
@@ -6126,8 +6126,8 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="78" zoomScaleNormal="78" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6152,7 +6152,7 @@
     </row>
     <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>1584</v>
+        <v>1582</v>
       </c>
       <c r="B2" s="46" t="s">
         <v>1423</v>
@@ -6179,10 +6179,10 @@
         <v>1420</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
@@ -6202,10 +6202,10 @@
         <v>1421</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -6275,7 +6275,7 @@
         <v>1429</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="E8" s="43" t="s">
         <v>318</v>
@@ -6292,7 +6292,7 @@
         <v>1430</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>1442</v>
+        <v>1440</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>409</v>
@@ -6309,7 +6309,7 @@
         <v>1431</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>1492</v>
+        <v>1490</v>
       </c>
       <c r="E10" s="43" t="s">
         <v>439</v>
@@ -6326,7 +6326,7 @@
         <v>1432</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>444</v>
@@ -6343,7 +6343,7 @@
         <v>1433</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="E12" s="22">
         <v>212</v>
@@ -6360,10 +6360,10 @@
         <v>1434</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>1477</v>
+        <v>1475</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6374,13 +6374,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>1439</v>
+        <v>1437</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>1482</v>
+        <v>1480</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="53" customHeight="1" x14ac:dyDescent="0.2">
@@ -6391,10 +6391,10 @@
         <v>3</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>1440</v>
+        <v>1438</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6405,13 +6405,13 @@
         <v>4</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>1435</v>
+        <v>1586</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6422,13 +6422,13 @@
         <v>7</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>1436</v>
+        <v>1585</v>
       </c>
       <c r="D17" s="43" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="E17" s="43" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
@@ -6439,10 +6439,10 @@
         <v>6</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>1437</v>
+        <v>1435</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
       <c r="E18" s="59" t="s">
         <v>441</v>
@@ -6450,16 +6450,16 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B19" s="60" t="s">
         <v>453</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="E19" s="62" t="s">
         <v>456</v>
@@ -6467,27 +6467,27 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B20" s="60" t="s">
         <v>438</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>1441</v>
+        <v>1439</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B21" s="60" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>1472</v>
+        <v>1470</v>
       </c>
       <c r="E21" s="43" t="s">
         <v>424</v>
@@ -6495,16 +6495,16 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B22" s="60" t="s">
         <v>431</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>1469</v>
+        <v>1467</v>
       </c>
       <c r="E22" s="22">
         <v>27565351</v>
@@ -6512,67 +6512,67 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B23" s="61" t="s">
         <v>405</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="D23" s="43" t="s">
-        <v>1470</v>
+        <v>1468</v>
       </c>
       <c r="E23" s="43" t="s">
-        <v>1471</v>
+        <v>1469</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B24" s="61" t="s">
         <v>451</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
       <c r="D24" s="43" t="s">
-        <v>1473</v>
+        <v>1471</v>
       </c>
       <c r="E24" s="56" t="s">
-        <v>1474</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B25" s="60" t="s">
         <v>433</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>1464</v>
+        <v>1462</v>
       </c>
       <c r="D25" s="43" t="s">
-        <v>1475</v>
+        <v>1473</v>
       </c>
       <c r="E25" s="43" t="s">
-        <v>1476</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B26" s="60" t="s">
         <v>450</v>
       </c>
       <c r="C26" s="48" t="s">
-        <v>1465</v>
+        <v>1463</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>1466</v>
+        <v>1464</v>
       </c>
       <c r="E26" s="43" t="s">
         <v>447</v>
@@ -6580,30 +6580,30 @@
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B27" s="61" t="s">
         <v>429</v>
       </c>
       <c r="C27" s="48" t="s">
-        <v>1467</v>
+        <v>1465</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>1468</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B28" s="60" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>1478</v>
+        <v>1476</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>1484</v>
+        <v>1482</v>
       </c>
       <c r="E28" s="43" t="s">
         <v>448</v>
@@ -6611,16 +6611,16 @@
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B29" s="60" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>1479</v>
+        <v>1477</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>1485</v>
+        <v>1483</v>
       </c>
       <c r="E29" s="43" t="s">
         <v>449</v>
@@ -6628,36 +6628,36 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B30" s="60" t="s">
         <v>452</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>1487</v>
+        <v>1485</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>1486</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B31" s="60" t="s">
         <v>434</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="D31" s="43" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="E31" s="43" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -6665,7 +6665,7 @@
     </row>
     <row r="33" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="46" t="s">
-        <v>1483</v>
+        <v>1481</v>
       </c>
       <c r="B33" s="46" t="s">
         <v>1423</v>
@@ -6694,13 +6694,13 @@
         <v>460</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>1493</v>
+        <v>1491</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>1527</v>
+        <v>1525</v>
       </c>
       <c r="E34" s="43" t="s">
-        <v>1528</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
@@ -6711,13 +6711,13 @@
         <v>458</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>1494</v>
+        <v>1492</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>1526</v>
+        <v>1524</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>1529</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6728,10 +6728,10 @@
         <v>461</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1585</v>
+        <v>1583</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="E36" s="43" t="s">
         <v>318</v>
@@ -6745,30 +6745,30 @@
         <v>486</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>1505</v>
+        <v>1503</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>1533</v>
+        <v>1531</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>1531</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="55" t="s">
-        <v>1530</v>
+        <v>1528</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>487</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>1506</v>
+        <v>1504</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>1534</v>
+        <v>1532</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>1532</v>
+        <v>1530</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6779,10 +6779,10 @@
         <v>459</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>1495</v>
+        <v>1493</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>1535</v>
+        <v>1533</v>
       </c>
       <c r="E39" s="43" t="s">
         <v>490</v>
@@ -6796,10 +6796,10 @@
         <v>470</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>1496</v>
+        <v>1494</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>1536</v>
+        <v>1534</v>
       </c>
       <c r="E40" s="43" t="s">
         <v>444</v>
@@ -6810,16 +6810,16 @@
         <v>1424</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>1586</v>
+        <v>1584</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>1537</v>
+        <v>1535</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>1559</v>
+        <v>1557</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -6830,10 +6830,10 @@
         <v>462</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>1497</v>
+        <v>1495</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>1538</v>
+        <v>1536</v>
       </c>
       <c r="E42" s="64" t="b">
         <v>1</v>
@@ -6847,10 +6847,10 @@
         <v>473</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>1581</v>
+        <v>1579</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>1539</v>
+        <v>1537</v>
       </c>
       <c r="E43" s="64" t="b">
         <v>0</v>
@@ -6864,10 +6864,10 @@
         <v>484</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>1498</v>
+        <v>1496</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>1540</v>
+        <v>1538</v>
       </c>
       <c r="E44" s="64" t="b">
         <v>1</v>
@@ -6881,10 +6881,10 @@
         <v>471</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>1499</v>
+        <v>1497</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>1541</v>
+        <v>1539</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>516</v>
@@ -6892,33 +6892,33 @@
     </row>
     <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B46" s="61" t="s">
         <v>1411</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="D46" s="43" t="s">
-        <v>1542</v>
+        <v>1540</v>
       </c>
       <c r="E46" s="67" t="s">
-        <v>1543</v>
+        <v>1541</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>1501</v>
+        <v>1499</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>1544</v>
+        <v>1542</v>
       </c>
       <c r="E47" s="68" t="s">
         <v>1414</v>
@@ -6926,84 +6926,84 @@
     </row>
     <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B48" s="61" t="s">
         <v>463</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>1502</v>
+        <v>1500</v>
       </c>
       <c r="D48" s="43" t="s">
-        <v>1545</v>
+        <v>1543</v>
       </c>
       <c r="E48" s="43" t="s">
-        <v>1546</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B49" s="61" t="s">
         <v>474</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>1503</v>
+        <v>1501</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1548</v>
+        <v>1546</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>1547</v>
+        <v>1545</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B50" s="61" t="s">
         <v>483</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>1504</v>
+        <v>1502</v>
       </c>
       <c r="D50" s="43" t="s">
-        <v>1551</v>
+        <v>1549</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>1549</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B51" s="61" t="s">
         <v>485</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>1507</v>
+        <v>1505</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>1550</v>
+        <v>1548</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>1554</v>
+        <v>1552</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B52" s="61" t="s">
         <v>452</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>1480</v>
+        <v>1478</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="E52" t="s">
         <v>1413</v>
@@ -7012,16 +7012,16 @@
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B53" s="61" t="s">
         <v>472</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>1508</v>
+        <v>1506</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>1553</v>
+        <v>1551</v>
       </c>
       <c r="E53" s="43" t="s">
         <v>1412</v>
@@ -7029,16 +7029,16 @@
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B54" s="61" t="s">
         <v>466</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>1509</v>
+        <v>1507</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>1555</v>
+        <v>1553</v>
       </c>
       <c r="E54" s="43" t="s">
         <v>509</v>
@@ -7046,16 +7046,16 @@
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B55" s="61" t="s">
         <v>478</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>1510</v>
+        <v>1508</v>
       </c>
       <c r="D55" s="43" t="s">
-        <v>1556</v>
+        <v>1554</v>
       </c>
       <c r="E55" s="64">
         <v>8.3000000000000007</v>
@@ -7063,231 +7063,231 @@
     </row>
     <row r="56" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B56" s="61" t="s">
         <v>464</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>1511</v>
+        <v>1509</v>
       </c>
       <c r="D56" s="43" t="s">
-        <v>1557</v>
+        <v>1555</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>1576</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B57" s="61" t="s">
         <v>465</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>1512</v>
+        <v>1510</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>1558</v>
+        <v>1556</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1577</v>
+        <v>1575</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B58" s="61" t="s">
         <v>475</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>1513</v>
+        <v>1511</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>1575</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B59" s="61" t="s">
         <v>434</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>1481</v>
+        <v>1479</v>
       </c>
       <c r="D59" s="43" t="s">
-        <v>1488</v>
+        <v>1486</v>
       </c>
       <c r="E59" s="43" t="s">
-        <v>1489</v>
+        <v>1487</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B60" s="61" t="s">
         <v>515</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>1514</v>
+        <v>1512</v>
       </c>
       <c r="D60" s="43" t="s">
-        <v>1578</v>
+        <v>1576</v>
       </c>
       <c r="E60" s="43" t="s">
-        <v>1579</v>
+        <v>1577</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B61" s="61" t="s">
         <v>482</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>1515</v>
+        <v>1513</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>1574</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B62" s="61" t="s">
         <v>467</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>1516</v>
+        <v>1514</v>
       </c>
       <c r="D62" s="43" t="s">
-        <v>1570</v>
+        <v>1568</v>
       </c>
       <c r="E62" s="43" t="s">
-        <v>1571</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B63" s="61" t="s">
         <v>480</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>1517</v>
+        <v>1515</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>1569</v>
+        <v>1567</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>1572</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B64" s="61" t="s">
         <v>514</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>1518</v>
+        <v>1516</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>1567</v>
+        <v>1565</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>1573</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B65" s="61" t="s">
         <v>476</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>1519</v>
+        <v>1517</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>1566</v>
+        <v>1564</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>1583</v>
+        <v>1581</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B66" s="61" t="s">
         <v>477</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>1520</v>
+        <v>1518</v>
       </c>
       <c r="D66" s="43" t="s">
-        <v>1560</v>
+        <v>1558</v>
       </c>
       <c r="E66" s="43" t="s">
-        <v>1561</v>
+        <v>1559</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B67" s="61" t="s">
         <v>479</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>1521</v>
+        <v>1519</v>
       </c>
       <c r="D67" s="43" t="s">
+        <v>1560</v>
+      </c>
+      <c r="E67" s="43" t="s">
         <v>1562</v>
-      </c>
-      <c r="E67" s="43" t="s">
-        <v>1564</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B68" s="61" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="C68" s="48" t="s">
-        <v>1523</v>
+        <v>1521</v>
       </c>
       <c r="D68" s="43" t="s">
-        <v>1568</v>
+        <v>1566</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>1563</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B69" s="61" t="s">
         <v>481</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>1524</v>
+        <v>1522</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>1580</v>
+        <v>1578</v>
       </c>
       <c r="E69" s="64">
         <v>20814</v>
@@ -7295,16 +7295,16 @@
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="55" t="s">
-        <v>1438</v>
+        <v>1436</v>
       </c>
       <c r="B70" s="61" t="s">
         <v>512</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>1525</v>
+        <v>1523</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>1565</v>
+        <v>1563</v>
       </c>
     </row>
   </sheetData>
@@ -7809,7 +7809,7 @@
         <v>470</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>462</v>
@@ -7984,7 +7984,7 @@
         <v>1411</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>463</v>
@@ -8047,7 +8047,7 @@
         <v>479</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>481</v>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44223</v>
+        <v>44351</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -8628,7 +8628,7 @@
         <v>470</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>462</v>
@@ -16740,7 +16740,7 @@
         <v>1411</v>
       </c>
       <c r="C218" s="32" t="s">
-        <v>1491</v>
+        <v>1489</v>
       </c>
       <c r="D218" s="15" t="s">
         <v>463</v>
@@ -16803,7 +16803,7 @@
         <v>479</v>
       </c>
       <c r="X218" s="2" t="s">
-        <v>1522</v>
+        <v>1520</v>
       </c>
       <c r="Y218" s="2" t="s">
         <v>481</v>
@@ -24262,7 +24262,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1582</v>
+        <v>1580</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>

</xml_diff>

<commit_message>
Adding new attribute "data_curator" to DME PI collection
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuhnsa/Desktop/Archive/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/pyrkit/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93188DA8-CE5D-334A-9143-EF0909ACDEF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0804DF8-8D4F-1C46-80EA-ABFA9988B233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23440" yWindow="-28340" windowWidth="35840" windowHeight="26680" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
@@ -4299,9 +4299,6 @@
   </si>
   <si>
     <t>Data Dictionary</t>
-  </si>
-  <si>
-    <t>pi_name</t>
   </si>
   <si>
     <t>affiliation</t>
@@ -5368,6 +5365,9 @@
   </si>
   <si>
     <t>project_start_date</t>
+  </si>
+  <si>
+    <t>data_owner</t>
   </si>
 </sst>
 </file>
@@ -6127,7 +6127,7 @@
   <dimension ref="A1:K70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6152,37 +6152,37 @@
     </row>
     <row r="2" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A2" s="46" t="s">
-        <v>1582</v>
+        <v>1581</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D2" s="47" t="s">
         <v>469</v>
       </c>
       <c r="E2" s="57" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="F2" s="50"/>
     </row>
     <row r="3" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B3" s="63" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>1420</v>
+        <v>1586</v>
       </c>
       <c r="D3" s="43" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="E3" s="43" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="F3" s="50"/>
       <c r="G3" s="50"/>
@@ -6193,19 +6193,19 @@
     </row>
     <row r="4" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B4" s="63" t="s">
         <v>403</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="D4" s="43" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="E4" s="58" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
@@ -6226,19 +6226,19 @@
     </row>
     <row r="6" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="46" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D6" s="47" t="s">
         <v>469</v>
       </c>
       <c r="E6" s="57" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="F6" s="52"/>
       <c r="G6" s="52"/>
@@ -6249,16 +6249,16 @@
     </row>
     <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>404</v>
       </c>
       <c r="C7" s="48" t="s">
+        <v>1426</v>
+      </c>
+      <c r="D7" s="43" t="s">
         <v>1427</v>
-      </c>
-      <c r="D7" s="43" t="s">
-        <v>1428</v>
       </c>
       <c r="E7" s="43" t="s">
         <v>13</v>
@@ -6266,16 +6266,16 @@
     </row>
     <row r="8" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B8" s="9" t="s">
         <v>408</v>
       </c>
       <c r="C8" s="48" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="D8" s="43" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="E8" s="43" t="s">
         <v>318</v>
@@ -6283,16 +6283,16 @@
     </row>
     <row r="9" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>432</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="D9" s="43" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="E9" s="43" t="s">
         <v>409</v>
@@ -6300,16 +6300,16 @@
     </row>
     <row r="10" spans="1:11" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="48" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="D10" s="43" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="E10" s="43" t="s">
         <v>439</v>
@@ -6317,16 +6317,16 @@
     </row>
     <row r="11" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>437</v>
       </c>
       <c r="C11" s="48" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="D11" s="43" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="E11" s="43" t="s">
         <v>444</v>
@@ -6334,16 +6334,16 @@
     </row>
     <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B12" s="25" t="s">
         <v>435</v>
       </c>
       <c r="C12" s="48" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="E12" s="22">
         <v>212</v>
@@ -6351,98 +6351,98 @@
     </row>
     <row r="13" spans="1:11" ht="136" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>436</v>
       </c>
       <c r="C13" s="48" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="D13" s="43" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="E13" s="43" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B14" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="D14" s="43" t="s">
-        <v>1461</v>
+        <v>1460</v>
       </c>
       <c r="E14" s="48" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="53" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="D15" s="43" t="s">
-        <v>1460</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C16" s="48" t="s">
-        <v>1586</v>
+        <v>1585</v>
       </c>
       <c r="D16" s="43" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="E16" s="43" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C17" s="48" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="D17" s="43" t="s">
+        <v>1446</v>
+      </c>
+      <c r="E17" s="43" t="s">
         <v>1447</v>
-      </c>
-      <c r="E17" s="43" t="s">
-        <v>1448</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="D18" s="43" t="s">
-        <v>1458</v>
+        <v>1457</v>
       </c>
       <c r="E18" s="59" t="s">
         <v>441</v>
@@ -6450,16 +6450,16 @@
     </row>
     <row r="19" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B19" s="60" t="s">
         <v>453</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="D19" s="43" t="s">
-        <v>1459</v>
+        <v>1458</v>
       </c>
       <c r="E19" s="62" t="s">
         <v>456</v>
@@ -6467,27 +6467,27 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B20" s="60" t="s">
         <v>438</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B21" s="60" t="s">
         <v>8</v>
       </c>
       <c r="C21" s="48" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="D21" s="43" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="E21" s="43" t="s">
         <v>424</v>
@@ -6495,16 +6495,16 @@
     </row>
     <row r="22" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B22" s="60" t="s">
         <v>431</v>
       </c>
       <c r="C22" s="48" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="D22" s="43" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="E22" s="22">
         <v>27565351</v>
@@ -6512,67 +6512,67 @@
     </row>
     <row r="23" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B23" s="61" t="s">
         <v>405</v>
       </c>
       <c r="C23" s="48" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="D23" s="43" t="s">
+        <v>1467</v>
+      </c>
+      <c r="E23" s="43" t="s">
         <v>1468</v>
-      </c>
-      <c r="E23" s="43" t="s">
-        <v>1469</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B24" s="61" t="s">
         <v>451</v>
       </c>
       <c r="C24" s="48" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="D24" s="43" t="s">
+        <v>1470</v>
+      </c>
+      <c r="E24" s="56" t="s">
         <v>1471</v>
-      </c>
-      <c r="E24" s="56" t="s">
-        <v>1472</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A25" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B25" s="60" t="s">
         <v>433</v>
       </c>
       <c r="C25" s="48" t="s">
-        <v>1462</v>
+        <v>1461</v>
       </c>
       <c r="D25" s="43" t="s">
+        <v>1472</v>
+      </c>
+      <c r="E25" s="43" t="s">
         <v>1473</v>
-      </c>
-      <c r="E25" s="43" t="s">
-        <v>1474</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B26" s="60" t="s">
         <v>450</v>
       </c>
       <c r="C26" s="48" t="s">
+        <v>1462</v>
+      </c>
+      <c r="D26" s="43" t="s">
         <v>1463</v>
-      </c>
-      <c r="D26" s="43" t="s">
-        <v>1464</v>
       </c>
       <c r="E26" s="43" t="s">
         <v>447</v>
@@ -6580,30 +6580,30 @@
     </row>
     <row r="27" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B27" s="61" t="s">
         <v>429</v>
       </c>
       <c r="C27" s="48" t="s">
+        <v>1464</v>
+      </c>
+      <c r="D27" s="43" t="s">
         <v>1465</v>
-      </c>
-      <c r="D27" s="43" t="s">
-        <v>1466</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B28" s="60" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="48" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="E28" s="43" t="s">
         <v>448</v>
@@ -6611,16 +6611,16 @@
     </row>
     <row r="29" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B29" s="60" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="48" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="E29" s="43" t="s">
         <v>449</v>
@@ -6628,36 +6628,36 @@
     </row>
     <row r="30" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B30" s="60" t="s">
         <v>452</v>
       </c>
       <c r="C30" s="48" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="E30" s="43" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A31" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B31" s="60" t="s">
         <v>434</v>
       </c>
       <c r="C31" s="48" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="D31" s="43" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E31" s="43" t="s">
         <v>1486</v>
-      </c>
-      <c r="E31" s="43" t="s">
-        <v>1487</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -6665,19 +6665,19 @@
     </row>
     <row r="33" spans="1:11" ht="20" x14ac:dyDescent="0.2">
       <c r="A33" s="46" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B33" s="46" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="D33" s="47" t="s">
         <v>469</v>
       </c>
       <c r="E33" s="57" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="F33" s="52"/>
       <c r="G33" s="52"/>
@@ -6688,50 +6688,50 @@
     </row>
     <row r="34" spans="1:11" ht="51" x14ac:dyDescent="0.2">
       <c r="A34" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B34" s="63" t="s">
         <v>460</v>
       </c>
       <c r="C34" s="48" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="D34" s="43" t="s">
+        <v>1524</v>
+      </c>
+      <c r="E34" s="43" t="s">
         <v>1525</v>
-      </c>
-      <c r="E34" s="43" t="s">
-        <v>1526</v>
       </c>
     </row>
     <row r="35" spans="1:11" ht="68" x14ac:dyDescent="0.2">
       <c r="A35" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B35" s="63" t="s">
         <v>458</v>
       </c>
       <c r="C35" s="48" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="D35" s="43" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="E35" s="43" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
     </row>
     <row r="36" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B36" s="63" t="s">
         <v>461</v>
       </c>
       <c r="C36" s="65" t="s">
-        <v>1583</v>
+        <v>1582</v>
       </c>
       <c r="D36" s="43" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="E36" s="43" t="s">
         <v>318</v>
@@ -6739,50 +6739,50 @@
     </row>
     <row r="37" spans="1:11" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B37" s="63" t="s">
         <v>486</v>
       </c>
       <c r="C37" s="48" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="D37" s="43" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="E37" s="43" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="55" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B38" s="63" t="s">
         <v>487</v>
       </c>
       <c r="C38" s="48" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="D38" s="43" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="E38" s="43" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B39" s="63" t="s">
         <v>459</v>
       </c>
       <c r="C39" s="48" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="D39" s="43" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="E39" s="43" t="s">
         <v>490</v>
@@ -6790,16 +6790,16 @@
     </row>
     <row r="40" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B40" s="63" t="s">
         <v>470</v>
       </c>
       <c r="C40" s="48" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="D40" s="43" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="E40" s="43" t="s">
         <v>444</v>
@@ -6807,33 +6807,33 @@
     </row>
     <row r="41" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B41" s="9" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="C41" s="48" t="s">
-        <v>1584</v>
+        <v>1583</v>
       </c>
       <c r="D41" s="43" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="E41" s="43" t="s">
-        <v>1557</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B42" s="63" t="s">
         <v>462</v>
       </c>
       <c r="C42" s="48" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="D42" s="43" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="E42" s="64" t="b">
         <v>1</v>
@@ -6841,16 +6841,16 @@
     </row>
     <row r="43" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B43" s="63" t="s">
         <v>473</v>
       </c>
       <c r="C43" s="48" t="s">
-        <v>1579</v>
+        <v>1578</v>
       </c>
       <c r="D43" s="43" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="E43" s="64" t="b">
         <v>0</v>
@@ -6858,16 +6858,16 @@
     </row>
     <row r="44" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B44" s="63" t="s">
         <v>484</v>
       </c>
       <c r="C44" s="48" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="D44" s="43" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="E44" s="64" t="b">
         <v>1</v>
@@ -6875,16 +6875,16 @@
     </row>
     <row r="45" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="51" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="B45" s="63" t="s">
         <v>471</v>
       </c>
       <c r="C45" s="48" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="D45" s="43" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="E45" s="43" t="s">
         <v>516</v>
@@ -6892,33 +6892,33 @@
     </row>
     <row r="46" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B46" s="61" t="s">
         <v>1411</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="D46" s="43" t="s">
+        <v>1539</v>
+      </c>
+      <c r="E46" s="67" t="s">
         <v>1540</v>
-      </c>
-      <c r="E46" s="67" t="s">
-        <v>1541</v>
       </c>
     </row>
     <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B47" s="61" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="C47" s="48" t="s">
-        <v>1499</v>
+        <v>1498</v>
       </c>
       <c r="D47" s="43" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="E47" s="68" t="s">
         <v>1414</v>
@@ -6926,84 +6926,84 @@
     </row>
     <row r="48" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B48" s="61" t="s">
         <v>463</v>
       </c>
       <c r="C48" s="48" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="D48" s="43" t="s">
+        <v>1542</v>
+      </c>
+      <c r="E48" s="43" t="s">
         <v>1543</v>
-      </c>
-      <c r="E48" s="43" t="s">
-        <v>1544</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B49" s="61" t="s">
         <v>474</v>
       </c>
       <c r="C49" s="48" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="D49" s="43" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="E49" s="64" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A50" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B50" s="61" t="s">
         <v>483</v>
       </c>
       <c r="C50" s="48" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="D50" s="43" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
       <c r="E50" s="43" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B51" s="61" t="s">
         <v>485</v>
       </c>
       <c r="C51" s="48" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="D51" s="43" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="E51" s="43" t="s">
-        <v>1552</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A52" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B52" s="61" t="s">
         <v>452</v>
       </c>
       <c r="C52" s="48" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="D52" s="43" t="s">
-        <v>1550</v>
+        <v>1549</v>
       </c>
       <c r="E52" t="s">
         <v>1413</v>
@@ -7012,16 +7012,16 @@
     </row>
     <row r="53" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A53" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B53" s="61" t="s">
         <v>472</v>
       </c>
       <c r="C53" s="48" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="D53" s="43" t="s">
-        <v>1551</v>
+        <v>1550</v>
       </c>
       <c r="E53" s="43" t="s">
         <v>1412</v>
@@ -7029,16 +7029,16 @@
     </row>
     <row r="54" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B54" s="61" t="s">
         <v>466</v>
       </c>
       <c r="C54" s="48" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="D54" s="43" t="s">
-        <v>1553</v>
+        <v>1552</v>
       </c>
       <c r="E54" s="43" t="s">
         <v>509</v>
@@ -7046,16 +7046,16 @@
     </row>
     <row r="55" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A55" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B55" s="61" t="s">
         <v>478</v>
       </c>
       <c r="C55" s="48" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="D55" s="43" t="s">
-        <v>1554</v>
+        <v>1553</v>
       </c>
       <c r="E55" s="64">
         <v>8.3000000000000007</v>
@@ -7063,231 +7063,231 @@
     </row>
     <row r="56" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B56" s="61" t="s">
         <v>464</v>
       </c>
       <c r="C56" s="48" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="D56" s="43" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="E56" s="43" t="s">
-        <v>1574</v>
+        <v>1573</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B57" s="61" t="s">
         <v>465</v>
       </c>
       <c r="C57" s="48" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="D57" s="43" t="s">
-        <v>1556</v>
+        <v>1555</v>
       </c>
       <c r="E57" s="43" t="s">
-        <v>1575</v>
+        <v>1574</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A58" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B58" s="61" t="s">
         <v>475</v>
       </c>
       <c r="C58" s="48" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="D58" s="43" t="s">
-        <v>1573</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A59" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B59" s="61" t="s">
         <v>434</v>
       </c>
       <c r="C59" s="48" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="D59" s="43" t="s">
+        <v>1485</v>
+      </c>
+      <c r="E59" s="43" t="s">
         <v>1486</v>
-      </c>
-      <c r="E59" s="43" t="s">
-        <v>1487</v>
       </c>
     </row>
     <row r="60" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B60" s="61" t="s">
         <v>515</v>
       </c>
       <c r="C60" s="48" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="D60" s="43" t="s">
+        <v>1575</v>
+      </c>
+      <c r="E60" s="43" t="s">
         <v>1576</v>
-      </c>
-      <c r="E60" s="43" t="s">
-        <v>1577</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B61" s="61" t="s">
         <v>482</v>
       </c>
       <c r="C61" s="48" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="D61" s="43" t="s">
-        <v>1572</v>
+        <v>1571</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B62" s="61" t="s">
         <v>467</v>
       </c>
       <c r="C62" s="48" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="D62" s="43" t="s">
+        <v>1567</v>
+      </c>
+      <c r="E62" s="43" t="s">
         <v>1568</v>
-      </c>
-      <c r="E62" s="43" t="s">
-        <v>1569</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B63" s="61" t="s">
         <v>480</v>
       </c>
       <c r="C63" s="48" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="D63" s="43" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
       <c r="E63" s="43" t="s">
-        <v>1570</v>
+        <v>1569</v>
       </c>
     </row>
     <row r="64" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B64" s="61" t="s">
         <v>514</v>
       </c>
       <c r="C64" s="48" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="D64" s="43" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
       <c r="E64" s="43" t="s">
-        <v>1571</v>
+        <v>1570</v>
       </c>
     </row>
     <row r="65" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A65" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B65" s="61" t="s">
         <v>476</v>
       </c>
       <c r="C65" s="48" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="D65" s="43" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
       <c r="E65" s="43" t="s">
-        <v>1581</v>
+        <v>1580</v>
       </c>
     </row>
     <row r="66" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B66" s="61" t="s">
         <v>477</v>
       </c>
       <c r="C66" s="48" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="D66" s="43" t="s">
+        <v>1557</v>
+      </c>
+      <c r="E66" s="43" t="s">
         <v>1558</v>
-      </c>
-      <c r="E66" s="43" t="s">
-        <v>1559</v>
       </c>
     </row>
     <row r="67" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B67" s="61" t="s">
         <v>479</v>
       </c>
       <c r="C67" s="48" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="D67" s="43" t="s">
-        <v>1560</v>
+        <v>1559</v>
       </c>
       <c r="E67" s="43" t="s">
-        <v>1562</v>
+        <v>1561</v>
       </c>
     </row>
     <row r="68" spans="1:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B68" s="61" t="s">
+        <v>1519</v>
+      </c>
+      <c r="C68" s="48" t="s">
         <v>1520</v>
       </c>
-      <c r="C68" s="48" t="s">
-        <v>1521</v>
-      </c>
       <c r="D68" s="43" t="s">
-        <v>1566</v>
+        <v>1565</v>
       </c>
       <c r="E68" s="43" t="s">
-        <v>1561</v>
+        <v>1560</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A69" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B69" s="61" t="s">
         <v>481</v>
       </c>
       <c r="C69" s="48" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="D69" s="43" t="s">
-        <v>1578</v>
+        <v>1577</v>
       </c>
       <c r="E69" s="64">
         <v>20814</v>
@@ -7295,16 +7295,16 @@
     </row>
     <row r="70" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="A70" s="55" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="B70" s="61" t="s">
         <v>512</v>
       </c>
       <c r="C70" s="48" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="D70" s="43" t="s">
-        <v>1563</v>
+        <v>1562</v>
       </c>
     </row>
   </sheetData>
@@ -7809,7 +7809,7 @@
         <v>470</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>462</v>
@@ -7984,7 +7984,7 @@
         <v>1411</v>
       </c>
       <c r="C36" s="32" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="D36" s="15" t="s">
         <v>463</v>
@@ -8047,7 +8047,7 @@
         <v>479</v>
       </c>
       <c r="X36" s="2" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="Y36" s="2" t="s">
         <v>481</v>
@@ -8263,7 +8263,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44351</v>
+        <v>44361</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -8628,7 +8628,7 @@
         <v>470</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="I3" s="29" t="s">
         <v>462</v>
@@ -16740,7 +16740,7 @@
         <v>1411</v>
       </c>
       <c r="C218" s="32" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="D218" s="15" t="s">
         <v>463</v>
@@ -16803,7 +16803,7 @@
         <v>479</v>
       </c>
       <c r="X218" s="2" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="Y218" s="2" t="s">
         <v>481</v>
@@ -24262,7 +24262,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1580</v>
+        <v>1579</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>

</xml_diff>

<commit_message>
Adding a new data provider
</commit_message>
<xml_diff>
--- a/data/experiment_metadata.xlsx
+++ b/data/experiment_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/pyrkit/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kuhnsa/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0804DF8-8D4F-1C46-80EA-ABFA9988B233}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7666384C-31AF-EC4A-9C4E-A868C762673C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23440" yWindow="-28340" windowWidth="35840" windowHeight="26680" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
+    <workbookView xWindow="-23640" yWindow="-27500" windowWidth="35840" windowHeight="26680" activeTab="1" xr2:uid="{A36FD966-9E32-3D40-B500-D853A176E406}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4375" uniqueCount="1587">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4377" uniqueCount="1589">
   <si>
     <t>PI Name</t>
   </si>
@@ -5368,6 +5368,12 @@
   </si>
   <si>
     <t>data_owner</t>
+  </si>
+  <si>
+    <t>KhanLab</t>
+  </si>
+  <si>
+    <t>Del Rivero, Jaydira</t>
   </si>
 </sst>
 </file>
@@ -6126,7 +6132,7 @@
   </sheetPr>
   <dimension ref="A1:K70"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
@@ -7325,7 +7331,7 @@
   </sheetPr>
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:D4"/>
     </sheetView>
   </sheetViews>
@@ -7652,18 +7658,6 @@
           </x14:formula1>
           <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{14B4FD48-719D-C048-A0EF-48D4AA60EEAF}">
-          <x14:formula1>
-            <xm:f>Options!$A$2:$A$301</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{60BD1DF6-F751-E148-9E9A-5F728055E719}">
-          <x14:formula1>
-            <xm:f>Options!$D$2:$D$18</xm:f>
-          </x14:formula1>
-          <xm:sqref>B9:D9</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{74CAC5C9-DEB1-4249-9509-C48D1A20D281}">
           <x14:formula1>
             <xm:f>Options!$E$2:$E$6</xm:f>
@@ -7681,6 +7675,18 @@
             <xm:f>Options!$C$2:$C$19</xm:f>
           </x14:formula1>
           <xm:sqref>C8:D8</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{60BD1DF6-F751-E148-9E9A-5F728055E719}">
+          <x14:formula1>
+            <xm:f>Options!$D$2:$D$19</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9:D9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{14B4FD48-719D-C048-A0EF-48D4AA60EEAF}">
+          <x14:formula1>
+            <xm:f>Options!$A$2:$A$302</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -8263,7 +8269,7 @@
       </c>
       <c r="B16" s="72">
         <f ca="1">TODAY()</f>
-        <v>44361</v>
+        <v>44384</v>
       </c>
       <c r="C16" s="72"/>
       <c r="D16" s="72"/>
@@ -8462,18 +8468,6 @@
           </x14:formula1>
           <xm:sqref>B23:C23</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{A1979415-C96C-6749-8339-A88C8FF73FE9}">
-          <x14:formula1>
-            <xm:f>Options!$D$2:$D$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>B9:C9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{AF0D3179-FB93-6C42-90C5-5BBA1913D1D1}">
-          <x14:formula1>
-            <xm:f>Options!$A$2:$A$301</xm:f>
-          </x14:formula1>
-          <xm:sqref>B4</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{D8189E72-C26C-1049-B3FC-08DEEED0E9E0}">
           <x14:formula1>
             <xm:f>Options!$B$2:$B$69</xm:f>
@@ -8498,11 +8492,23 @@
           </x14:formula1>
           <xm:sqref>D8</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{A1979415-C96C-6749-8339-A88C8FF73FE9}">
+          <x14:formula1>
+            <xm:f>Options!$D$2:$D$18</xm:f>
+          </x14:formula1>
+          <xm:sqref>B9:C9</xm:sqref>
+        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{6A52EF0B-008C-3B44-B7B5-201D83C2DF37}">
           <x14:formula1>
-            <xm:f>Options!$D$2:$D$17</xm:f>
+            <xm:f>Options!$D$2:$D$18</xm:f>
           </x14:formula1>
           <xm:sqref>D9</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{AF0D3179-FB93-6C42-90C5-5BBA1913D1D1}">
+          <x14:formula1>
+            <xm:f>Options!$A$2:$A$302</xm:f>
+          </x14:formula1>
+          <xm:sqref>B4</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -23933,10 +23939,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{330CACDC-8C65-0842-9840-2AAC530055D5}">
-  <dimension ref="A1:K301"/>
+  <dimension ref="A1:K302"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -24161,7 +24167,7 @@
         <v>454</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>411</v>
+        <v>1587</v>
       </c>
       <c r="E7" s="3"/>
       <c r="G7" s="3" t="s">
@@ -24182,7 +24188,7 @@
         <v>318</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E8" s="3"/>
       <c r="G8" s="3" t="s">
@@ -24203,7 +24209,7 @@
         <v>324</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="E9" s="3"/>
       <c r="G9" s="3" t="s">
@@ -24224,7 +24230,7 @@
         <v>320</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="E10" s="3"/>
       <c r="G10" s="3"/>
@@ -24243,7 +24249,7 @@
         <v>319</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="E11" s="3"/>
       <c r="G11" s="3"/>
@@ -24262,7 +24268,7 @@
         <v>330</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>1579</v>
+        <v>415</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="23"/>
@@ -24281,7 +24287,7 @@
         <v>331</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>416</v>
+        <v>1579</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="23"/>
@@ -24300,7 +24306,7 @@
         <v>317</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="23"/>
@@ -24319,7 +24325,7 @@
         <v>323</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E15" s="3"/>
     </row>
@@ -24334,7 +24340,7 @@
         <v>325</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -24349,7 +24355,7 @@
         <v>322</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="E17" s="3"/>
     </row>
@@ -24364,7 +24370,7 @@
         <v>326</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -24377,6 +24383,9 @@
       <c r="C19" s="3" t="s">
         <v>327</v>
       </c>
+      <c r="D19" s="3" t="s">
+        <v>423</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
@@ -24708,7 +24717,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
-        <v>72</v>
+        <v>1588</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>390</v>
@@ -24716,7 +24725,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B62" s="3" t="s">
         <v>391</v>
@@ -24724,7 +24733,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B63" s="3" t="s">
         <v>392</v>
@@ -24732,7 +24741,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>393</v>
@@ -24740,7 +24749,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>394</v>
@@ -24748,7 +24757,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>395</v>
@@ -24756,7 +24765,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B67" s="3" t="s">
         <v>396</v>
@@ -24764,7 +24773,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B68" s="3" t="s">
         <v>397</v>
@@ -24772,7 +24781,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69" s="3" t="s">
         <v>398</v>
@@ -24780,1161 +24789,1166 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A118" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A120" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A121" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A122" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A123" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A125" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A126" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A127" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A128" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A129" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A130" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A131" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A132" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A137" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A138" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A139" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A140" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A141" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A142" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A143" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A144" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A145" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A146" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A147" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A148" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A149" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A151" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A152" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A153" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A154" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A155" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A156" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A158" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A159" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A160" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A177" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A178" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A179" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A180" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A181" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A182" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A183" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A184" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A185" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A188" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A189" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="190" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A191" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A192" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A193" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A194" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A195" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A196" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="197" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A197" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A199" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A200" s="3" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A201" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A202" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A203" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A204" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="205" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A205" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A206" s="3" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A207" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A208" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A209" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A210" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A211" s="3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A212" s="3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="213" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A213" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="214" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A214" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A215" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="216" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A216" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A217" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A218" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A219" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A221" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A222" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A223" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="224" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A225" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A229" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A230" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A231" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="232" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A232" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A233" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A234" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A235" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A236" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A237" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A238" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A239" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="240" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A240" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A241" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A242" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A243" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A244" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A245" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A246" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A247" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="248" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A248" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A249" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A250" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A251" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A252" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A253" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A254" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A255" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="256" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A256" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A257" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A258" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A259" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A260" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A261" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A262" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A263" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="264" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A264" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="265" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A265" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A266" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="267" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A267" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A268" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A269" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A270" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A271" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A272" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A273" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="274" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A274" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A275" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A276" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A277" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A278" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A279" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A280" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="281" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A281" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A282" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A283" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A284" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A285" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A286" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A287" s="3" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="288" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A288" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A289" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A290" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A291" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A292" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A293" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A294" s="3" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="295" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A295" s="3" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A296" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A297" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A298" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A299" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A300" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="302" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A302" s="3" t="s">
         <v>312</v>
       </c>
     </row>

</xml_diff>